<commit_message>
IPPU model complete. Garbage data template completed for IPPU.
</commit_message>
<xml_diff>
--- a/ref/ingestion/parameters_demo/model_input_variables_ce_demo.xlsx
+++ b/ref/ingestion/parameters_demo/model_input_variables_ce_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/ingestion/parameters_demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56AC3FA-50FA-684F-9B58-8D117015DCF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60AD21C0-88EE-4645-9491-88DE616B7777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11080" yWindow="3240" windowWidth="23800" windowHeight="20820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5820" yWindow="460" windowWidth="34660" windowHeight="20820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="strategy_id-0" sheetId="1" r:id="rId1"/>
@@ -1144,8 +1144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I99" sqref="I99"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -23504,8 +23504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AS1"/>
   <sheetViews>
-    <sheetView topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="T30" sqref="T30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added Industrial Energy and updated some files
</commit_message>
<xml_diff>
--- a/ref/ingestion/parameters_demo/model_input_variables_ce_demo.xlsx
+++ b/ref/ingestion/parameters_demo/model_input_variables_ce_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/ingestion/parameters_demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60AD21C0-88EE-4645-9491-88DE616B7777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD28AC6-2147-1849-BD96-BDBD791EAE9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5820" yWindow="460" windowWidth="34660" windowHeight="20820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1580" yWindow="1100" windowWidth="34660" windowHeight="20620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="strategy_id-0" sheetId="1" r:id="rId1"/>
@@ -1144,8 +1144,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="207" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U42" sqref="U42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added Stationary Combustion and Other Energy
</commit_message>
<xml_diff>
--- a/ref/ingestion/parameters_demo/model_input_variables_ce_demo.xlsx
+++ b/ref/ingestion/parameters_demo/model_input_variables_ce_demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/ingestion/parameters_demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48973758-2C88-0B41-954C-11B453D951DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C0CD62-D00A-ED4B-A8C1-D905C15AAB53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="460" windowWidth="34660" windowHeight="20620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1178,8 +1178,8 @@
   <dimension ref="A1:AS194"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="207" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H155" sqref="H155"/>
+      <pane ySplit="1" topLeftCell="A138" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O179" sqref="O179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Completed IPPU with new fake data, templates, attribute table, scripts, and calibraiton ino
</commit_message>
<xml_diff>
--- a/ref/ingestion/parameters_demo/model_input_variables_ce_demo.xlsx
+++ b/ref/ingestion/parameters_demo/model_input_variables_ce_demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/ingestion/parameters_demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18375B37-C990-3F4B-B772-7561534F6383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592DD241-A119-3B46-8E69-DEA6637EF5E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3080" yWindow="460" windowWidth="28960" windowHeight="20620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8060" yWindow="460" windowWidth="28960" windowHeight="20620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="strategy_id-0" sheetId="1" r:id="rId1"/>
@@ -1288,9 +1288,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS226"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="207" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I118" sqref="I118"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="75" zoomScaleNormal="207" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AS137" sqref="AS137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated calibration matrix for IPPU
</commit_message>
<xml_diff>
--- a/ref/ingestion/parameters_demo/model_input_variables_ce_demo.xlsx
+++ b/ref/ingestion/parameters_demo/model_input_variables_ce_demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/ingestion/parameters_demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592DD241-A119-3B46-8E69-DEA6637EF5E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E023094B-0165-E84D-8775-40A0407E713C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8060" yWindow="460" windowWidth="28960" windowHeight="20620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1288,9 +1288,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="75" zoomScaleNormal="207" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AS137" sqref="AS137"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="207" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Y142" sqref="Y142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
completed chain and energy models, updated run_sector_models.py
</commit_message>
<xml_diff>
--- a/ref/ingestion/parameters_demo/model_input_variables_ce_demo.xlsx
+++ b/ref/ingestion/parameters_demo/model_input_variables_ce_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jsyme/Documents/Projects/git_jbus/lac_decarbonization/ref/ingestion/parameters_demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E023094B-0165-E84D-8775-40A0407E713C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29E61E5-4778-D147-921F-F95DBAB8689D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8060" yWindow="460" windowWidth="28960" windowHeight="20620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6880" yWindow="460" windowWidth="28960" windowHeight="20620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="strategy_id-0" sheetId="1" r:id="rId1"/>
@@ -1289,8 +1289,8 @@
   <dimension ref="A1:AS226"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="207" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y142" sqref="Y142"/>
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B134" sqref="B134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>